<commit_message>
Tratamiento Especial de Variables
Se avanza en el tratamiento de variables especiales
</commit_message>
<xml_diff>
--- a/Support Files/Tratamiento a Variables.xlsx
+++ b/Support Files/Tratamiento a Variables.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mardo\Documents\Repositories\Proyecto-Polifenoles\Support Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C42E8705-C581-42F1-B13E-02C4C1CC8DDD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1139D506-A59E-43CE-BCFC-05EE147EC986}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-1020" windowWidth="29040" windowHeight="15720" activeTab="3" xr2:uid="{034F1915-4034-48EB-BB58-54D0E05D6A98}"/>
   </bookViews>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="718" uniqueCount="684">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="719" uniqueCount="685">
   <si>
     <t>frec_alcohol_audit</t>
   </si>
@@ -2113,6 +2113,9 @@
       </rPr>
       <t>'total_meds'</t>
     </r>
+  </si>
+  <si>
+    <t>PENDIENTE APLICAR LA FUNCIÓN DE RELLENAR</t>
   </si>
 </sst>
 </file>
@@ -2157,12 +2160,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -2177,7 +2186,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -2191,11 +2200,11 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -2206,9 +2215,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -8013,8 +8026,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A05DF8D6-FC28-42E3-A215-A4BF25D82B23}">
   <dimension ref="A1:F43"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9:D10"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8029,7 +8042,7 @@
       <c r="A1" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B1" s="6" t="s">
+      <c r="B1" s="5" t="s">
         <v>7</v>
       </c>
       <c r="D1" s="4" t="s">
@@ -8058,7 +8071,7 @@
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="10" t="s">
+      <c r="A3" s="6" t="s">
         <v>683</v>
       </c>
       <c r="B3" s="3" t="s">
@@ -8142,15 +8155,19 @@
       </c>
     </row>
     <row r="11" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A11" s="5" t="s">
+      <c r="A11" s="10" t="s">
         <v>279</v>
       </c>
-      <c r="B11" s="3" t="s">
+      <c r="B11" s="11" t="s">
         <v>278</v>
       </c>
+      <c r="C11" s="12"/>
       <c r="D11" s="1" t="str">
         <f t="shared" si="0"/>
         <v>- num_depo</v>
+      </c>
+      <c r="E11" t="s">
+        <v>684</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">

</xml_diff>